<commit_message>
finished all data, fixed typos, reran all statistics
</commit_message>
<xml_diff>
--- a/Nemenyi-Cross-Temporal.xlsx
+++ b/Nemenyi-Cross-Temporal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Research/WindPowerForecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="357" documentId="8_{63ADE94E-410A-4C0D-8F01-08D87F8CF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{747BB297-4AFE-4C02-907C-BD6E382E8B3F}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{63ADE94E-410A-4C0D-8F01-08D87F8CF346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83388EDA-0FB6-4BE0-BC80-3EEB690D5CC8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EEDB9E72-6745-43F5-85AB-BC96E2F495CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EEDB9E72-6745-43F5-85AB-BC96E2F495CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,8 +132,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,13 +169,324 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -389,10 +708,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,37 +1009,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD089331-65FA-4BE0-B0F3-2D07DA26ECA7}">
   <dimension ref="A1:AO124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123:AB124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" customWidth="1"/>
+    <col min="8" max="8" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -810,7 +1125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.01954223361298</v>
       </c>
@@ -896,7 +1211,7 @@
         <v>0.96951317244848101</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.0353880826804001</v>
       </c>
@@ -982,7 +1297,7 @@
         <v>0.95747620262741895</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.0140937313563201</v>
       </c>
@@ -1068,7 +1383,7 @@
         <v>0.95479965029871505</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.02772956820254</v>
       </c>
@@ -1154,7 +1469,7 @@
         <v>0.96533874948224796</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.0415213213802399</v>
       </c>
@@ -1240,7 +1555,7 @@
         <v>0.96258112105599303</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.04059017949423</v>
       </c>
@@ -1326,7 +1641,7 @@
         <v>0.98325859174786201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.0437192318040101</v>
       </c>
@@ -1412,7 +1727,7 @@
         <v>0.93432706502128604</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.04901335616485</v>
       </c>
@@ -1498,7 +1813,7 @@
         <v>0.96576340217941004</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1.0459984597429199</v>
       </c>
@@ -1584,7 +1899,7 @@
         <v>0.96600798035576296</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1.0434423728145401</v>
       </c>
@@ -1670,7 +1985,7 @@
         <v>0.95521933044057095</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1.0563707945843499</v>
       </c>
@@ -1756,7 +2071,7 @@
         <v>0.97081862178101797</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1.0452483765243299</v>
       </c>
@@ -1842,7 +2157,7 @@
         <v>0.95559599694148001</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1.03743694485446</v>
       </c>
@@ -1928,7 +2243,7 @@
         <v>0.96184791134586201</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1.0336054317727901</v>
       </c>
@@ -2014,7 +2329,7 @@
         <v>0.96953713214411297</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1.0284835421280101</v>
       </c>
@@ -2100,7 +2415,7 @@
         <v>0.968356535809483</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1.0250487504525001</v>
       </c>
@@ -2186,7 +2501,7 @@
         <v>0.94993460485296599</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1.0196706368705799</v>
       </c>
@@ -2272,7 +2587,7 @@
         <v>0.96641808282728803</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1.0427471428521</v>
       </c>
@@ -2358,7 +2673,7 @@
         <v>0.98107892408068897</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1.00876995379965</v>
       </c>
@@ -2444,7 +2759,7 @@
         <v>0.95584132275947997</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1.01613150186537</v>
       </c>
@@ -2530,7 +2845,7 @@
         <v>0.95489899103022602</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1.0491326959332401</v>
       </c>
@@ -2616,7 +2931,7 @@
         <v>0.95878665769396298</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1.0364346832235001</v>
       </c>
@@ -2702,7 +3017,7 @@
         <v>0.96847881938572</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1.0248355873107999</v>
       </c>
@@ -2788,7 +3103,7 @@
         <v>0.96674848181954298</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1.02615855605854</v>
       </c>
@@ -2874,7 +3189,7 @@
         <v>0.96954156187443297</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1.0532476771888</v>
       </c>
@@ -2960,7 +3275,7 @@
         <v>0.96839567686330996</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1.0450997602563401</v>
       </c>
@@ -3046,7 +3361,7 @@
         <v>0.96181731345212595</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1.0657547210198099</v>
       </c>
@@ -3132,7 +3447,7 @@
         <v>0.98191146079418701</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1.0512504458460801</v>
       </c>
@@ -3218,7 +3533,7 @@
         <v>0.97042105359471198</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1.07271990476144</v>
       </c>
@@ -3304,7 +3619,7 @@
         <v>0.965109484162612</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1.0618323376733101</v>
       </c>
@@ -3390,7 +3705,7 @@
         <v>0.96151720716231803</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1.02254900769569</v>
       </c>
@@ -3476,7 +3791,7 @@
         <v>0.95406134798004105</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1.04661780582252</v>
       </c>
@@ -3562,7 +3877,7 @@
         <v>0.94349030347273699</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1.0177594459541499</v>
       </c>
@@ -3648,7 +3963,7 @@
         <v>0.93143643709589496</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1.0307712227397501</v>
       </c>
@@ -3734,7 +4049,7 @@
         <v>0.95763004386452999</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1.0434980180059901</v>
       </c>
@@ -3820,7 +4135,7 @@
         <v>0.95000424378298498</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1.0442772122580499</v>
       </c>
@@ -3906,7 +4221,7 @@
         <v>0.96165337180777999</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1.0536164819135201</v>
       </c>
@@ -3992,7 +4307,7 @@
         <v>0.94485556580915797</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1.0416683100597299</v>
       </c>
@@ -4078,7 +4393,7 @@
         <v>0.94267098948224304</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1.05286234355721</v>
       </c>
@@ -4164,7 +4479,7 @@
         <v>0.95474336438606</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1.04997922138813</v>
       </c>
@@ -4250,7 +4565,7 @@
         <v>0.94544642153448899</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1.0771596475154099</v>
       </c>
@@ -4336,7 +4651,7 @@
         <v>0.96223157008610505</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1.0582776013922399</v>
       </c>
@@ -4422,7 +4737,7 @@
         <v>0.94115440096617398</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1.04290932176031</v>
       </c>
@@ -4508,7 +4823,7 @@
         <v>0.94914560603196896</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1.0374560941669699</v>
       </c>
@@ -4594,7 +4909,7 @@
         <v>0.94791991505641304</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1.03033737335958</v>
       </c>
@@ -4680,7 +4995,7 @@
         <v>0.93262503881611403</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1.02441193912605</v>
       </c>
@@ -4766,7 +5081,7 @@
         <v>0.92230133652748503</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1.0246542787639299</v>
       </c>
@@ -4852,7 +5167,7 @@
         <v>0.94336578503870705</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1.0406298812268999</v>
       </c>
@@ -4938,7 +5253,7 @@
         <v>0.95182122312936301</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1.02482797499638</v>
       </c>
@@ -5024,7 +5339,7 @@
         <v>0.94812004350441104</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1.03842909193399</v>
       </c>
@@ -5110,7 +5425,7 @@
         <v>0.94619245499652405</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1.07067836491916</v>
       </c>
@@ -5196,7 +5511,7 @@
         <v>0.96187859250770802</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1.0491667902774999</v>
       </c>
@@ -5282,7 +5597,7 @@
         <v>0.96588305797804497</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1.0338646770461899</v>
       </c>
@@ -5368,7 +5683,7 @@
         <v>0.96996835118452795</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1.02533728782444</v>
       </c>
@@ -5454,7 +5769,7 @@
         <v>0.95161109684737299</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1.0606948216138099</v>
       </c>
@@ -5540,7 +5855,7 @@
         <v>0.96433365223665701</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1.0621225256138001</v>
       </c>
@@ -5626,7 +5941,7 @@
         <v>0.961716412319776</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1.05972025424886</v>
       </c>
@@ -5712,7 +6027,7 @@
         <v>0.96017178023740501</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1.05721473547378</v>
       </c>
@@ -5798,7 +6113,7 @@
         <v>0.97144235257113198</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1.0757958083068999</v>
       </c>
@@ -5884,7 +6199,7 @@
         <v>0.95487519194645198</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1.05759230979996</v>
       </c>
@@ -5970,7 +6285,7 @@
         <v>0.94755106920544896</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1.0095656598473799</v>
       </c>
@@ -6056,7 +6371,7 @@
         <v>0.904482688104712</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1.0520944471562601</v>
       </c>
@@ -6142,7 +6457,7 @@
         <v>0.90745018748992801</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1.0126666420660599</v>
       </c>
@@ -6228,7 +6543,7 @@
         <v>0.88605863691389897</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1.0338569453440001</v>
       </c>
@@ -6314,7 +6629,7 @@
         <v>0.92603218216597705</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1.0348657258892999</v>
       </c>
@@ -6400,7 +6715,7 @@
         <v>0.91451362474255704</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1.04547458295179</v>
       </c>
@@ -6486,7 +6801,7 @@
         <v>0.92827718203066101</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1.06580309587</v>
       </c>
@@ -6572,7 +6887,7 @@
         <v>0.93774761680880203</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1.0455438107894</v>
       </c>
@@ -6658,7 +6973,7 @@
         <v>0.90740097315451795</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1.0534524966088701</v>
       </c>
@@ -6744,7 +7059,7 @@
         <v>0.92105901570668003</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1.05675913561711</v>
       </c>
@@ -6830,7 +7145,7 @@
         <v>0.91608719065320499</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1.0750213519087699</v>
       </c>
@@ -6916,7 +7231,7 @@
         <v>0.93094252923092202</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1.0632872150205901</v>
       </c>
@@ -7002,7 +7317,7 @@
         <v>0.90524037512100497</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1.03109019959069</v>
       </c>
@@ -7088,7 +7403,7 @@
         <v>0.91305374550284402</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1.0340827684824001</v>
       </c>
@@ -7174,7 +7489,7 @@
         <v>0.90790511322155998</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1.0336475202442901</v>
       </c>
@@ -7260,7 +7575,7 @@
         <v>0.90971149811963203</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1.01830153627376</v>
       </c>
@@ -7346,7 +7661,7 @@
         <v>0.88612559374364597</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1.02235818279598</v>
       </c>
@@ -7432,7 +7747,7 @@
         <v>0.90798742305644797</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1.0335138380086499</v>
       </c>
@@ -7518,7 +7833,7 @@
         <v>0.91279210617953899</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1.01548567603489</v>
       </c>
@@ -7604,7 +7919,7 @@
         <v>0.91256456634538197</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1.0366836890014799</v>
       </c>
@@ -7690,7 +8005,7 @@
         <v>0.91704060187651903</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1.0636802859066701</v>
       </c>
@@ -7776,7 +8091,7 @@
         <v>0.92207660767793598</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1.04924321854866</v>
       </c>
@@ -7862,7 +8177,7 @@
         <v>0.93799261657997501</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1.0363282710995001</v>
       </c>
@@ -7948,7 +8263,7 @@
         <v>0.94599315582437105</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1.0275652645506399</v>
       </c>
@@ -8034,7 +8349,7 @@
         <v>0.922441898548642</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1.06342384762855</v>
       </c>
@@ -8120,7 +8435,7 @@
         <v>0.92584933577108997</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1.05927279350352</v>
       </c>
@@ -8206,7 +8521,7 @@
         <v>0.93874850831334</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1.05831281029714</v>
       </c>
@@ -8292,7 +8607,7 @@
         <v>0.92043443260039104</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1.0558735593189601</v>
       </c>
@@ -8378,7 +8693,7 @@
         <v>0.94090790141493996</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1.06876081204923</v>
       </c>
@@ -8464,7 +8779,7 @@
         <v>0.92377304142786698</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1.0511086357964301</v>
       </c>
@@ -8550,7 +8865,7 @@
         <v>0.90925447717791597</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.98580504083140097</v>
       </c>
@@ -8636,7 +8951,7 @@
         <v>0.76733762675568395</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1.02746312109946</v>
       </c>
@@ -8722,7 +9037,7 @@
         <v>0.80417958085961605</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1.00130815344761</v>
       </c>
@@ -8808,7 +9123,7 @@
         <v>0.77959765297837103</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1.01664716613923</v>
       </c>
@@ -8894,7 +9209,7 @@
         <v>0.80897426156552099</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1.0263586381618599</v>
       </c>
@@ -8980,7 +9295,7 @@
         <v>0.80193512025889502</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1.0286434246142899</v>
       </c>
@@ -9066,7 +9381,7 @@
         <v>0.82599755760751803</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1.0447327925936201</v>
       </c>
@@ -9152,7 +9467,7 @@
         <v>0.87713892652396597</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>1.03122805923482</v>
       </c>
@@ -9238,7 +9553,7 @@
         <v>0.79707651563509696</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1.0403985616481499</v>
       </c>
@@ -9324,7 +9639,7 @@
         <v>0.82887201062593097</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1.0473166651355701</v>
       </c>
@@ -9410,7 +9725,7 @@
         <v>0.82580733273495099</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1.05033919938249</v>
       </c>
@@ -9496,7 +9811,7 @@
         <v>0.84293689940257299</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1.0371047387700401</v>
       </c>
@@ -9582,7 +9897,7 @@
         <v>0.81116046234016903</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1.0174832967782499</v>
       </c>
@@ -9668,7 +9983,7 @@
         <v>0.82027989941616297</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1.01715645355712</v>
       </c>
@@ -9754,7 +10069,7 @@
         <v>0.81356224941130795</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1.0120410167812799</v>
       </c>
@@ -9840,7 +10155,7 @@
         <v>0.81848671340299906</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1.0165771098854699</v>
       </c>
@@ -9926,7 +10241,7 @@
         <v>0.80567064772669506</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>1.0091011985537</v>
       </c>
@@ -10012,7 +10327,7 @@
         <v>0.82049289250875101</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1.0198068818472901</v>
       </c>
@@ -10098,7 +10413,7 @@
         <v>0.81573056622228401</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1.02065988512823</v>
       </c>
@@ -10184,7 +10499,7 @@
         <v>0.82210870210675102</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1.01547195304612</v>
       </c>
@@ -10270,7 +10585,7 @@
         <v>0.81918898602768797</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1.0365885612886501</v>
       </c>
@@ -10356,7 +10671,7 @@
         <v>0.80681450447906899</v>
       </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1.02653953921513</v>
       </c>
@@ -10442,7 +10757,7 @@
         <v>0.82829555180324999</v>
       </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>1.0205423283936901</v>
       </c>
@@ -10528,7 +10843,7 @@
         <v>0.83746949482641597</v>
       </c>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1.0096993035433099</v>
       </c>
@@ -10614,7 +10929,7 @@
         <v>0.81412268151829303</v>
       </c>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1.0599678438170801</v>
       </c>
@@ -10700,7 +11015,7 @@
         <v>0.82250518331324796</v>
       </c>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1.04585006826004</v>
       </c>
@@ -10786,7 +11101,7 @@
         <v>0.84313933175242595</v>
       </c>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1.03021729381727</v>
       </c>
@@ -10872,7 +11187,7 @@
         <v>0.81206426150662803</v>
       </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1.0454317917292899</v>
       </c>
@@ -10958,7 +11273,7 @@
         <v>0.83656683436365897</v>
       </c>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1.04715410037977</v>
       </c>
@@ -11044,7 +11359,7 @@
         <v>0.82617140370078501</v>
       </c>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1.0368747482804199</v>
       </c>
@@ -11130,7 +11445,7 @@
         <v>0.79350685312700997</v>
       </c>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.35">
       <c r="AN122">
         <f>GEOMEAN(AB2:AB121)</f>
         <v>0.910735747193682</v>
@@ -11139,63 +11454,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="O123">
-        <f t="shared" ref="C123:AB123" si="0">GEOMEAN(O2:O121)</f>
-        <v>0.96601105415054256</v>
-      </c>
-      <c r="P123">
-        <f t="shared" si="0"/>
-        <v>0.93907253709256522</v>
-      </c>
-      <c r="Q123">
-        <f t="shared" si="0"/>
-        <v>0.9099989366025375</v>
-      </c>
-      <c r="R123">
-        <f t="shared" si="0"/>
-        <v>0.91873082455939248</v>
-      </c>
-      <c r="S123">
-        <f t="shared" si="0"/>
-        <v>0.91876084931921909</v>
-      </c>
-      <c r="T123">
-        <f t="shared" si="0"/>
-        <v>0.90912104547790806</v>
-      </c>
-      <c r="U123">
-        <f t="shared" si="0"/>
-        <v>0.90868239682633578</v>
-      </c>
-      <c r="V123">
-        <f t="shared" si="0"/>
-        <v>0.9723949967518345</v>
-      </c>
-      <c r="W123">
-        <f t="shared" si="0"/>
-        <v>0.93791384467132943</v>
-      </c>
-      <c r="X123">
-        <f t="shared" si="0"/>
-        <v>0.91598719373175652</v>
-      </c>
-      <c r="Y123">
-        <f t="shared" si="0"/>
-        <v>0.92619240109850387</v>
-      </c>
-      <c r="Z123">
-        <f t="shared" si="0"/>
-        <v>0.92548915621322325</v>
-      </c>
-      <c r="AA123">
-        <f t="shared" si="0"/>
-        <v>0.91402924482871917</v>
-      </c>
-      <c r="AB123">
-        <f t="shared" si="0"/>
-        <v>0.910735747193682</v>
-      </c>
+    <row r="123" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="O123" s="1"/>
       <c r="AN123">
         <f>AVERAGE(AB2:AB121)</f>
         <v>0.91273981380369673</v>
@@ -11204,89 +11464,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="O124">
-        <f t="shared" ref="C124:AB124" si="1">AVERAGE(O2:O121)</f>
-        <v>0.96606704613843764</v>
-      </c>
-      <c r="P124">
-        <f t="shared" si="1"/>
-        <v>0.94074928922239009</v>
-      </c>
-      <c r="Q124">
-        <f t="shared" si="1"/>
-        <v>0.91184507609058085</v>
-      </c>
-      <c r="R124">
-        <f t="shared" si="1"/>
-        <v>0.92050817450229694</v>
-      </c>
-      <c r="S124">
-        <f t="shared" si="1"/>
-        <v>0.92053767295165112</v>
-      </c>
-      <c r="T124">
-        <f t="shared" si="1"/>
-        <v>0.91097296858513743</v>
-      </c>
-      <c r="U124">
-        <f t="shared" si="1"/>
-        <v>0.9105581210579482</v>
-      </c>
-      <c r="V124">
-        <f t="shared" si="1"/>
-        <v>0.97245016447544685</v>
-      </c>
-      <c r="W124">
-        <f t="shared" si="1"/>
-        <v>0.93968011710813115</v>
-      </c>
-      <c r="X124">
-        <f t="shared" si="1"/>
-        <v>0.91790926563136765</v>
-      </c>
-      <c r="Y124">
-        <f t="shared" si="1"/>
-        <v>0.92803930449213501</v>
-      </c>
-      <c r="Z124">
-        <f t="shared" si="1"/>
-        <v>0.92733820537364697</v>
-      </c>
-      <c r="AA124">
-        <f t="shared" si="1"/>
-        <v>0.91595201234611001</v>
-      </c>
-      <c r="AB124">
-        <f t="shared" si="1"/>
-        <v>0.91273981380369673</v>
-      </c>
+    <row r="124" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="O124" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S28 H28:M28 A28:E28">
-    <cfRule type="top10" dxfId="14" priority="8" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S29 H29:M29 A29:E29">
-    <cfRule type="top10" dxfId="13" priority="7" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30 H30:M30 A30:E30">
-    <cfRule type="top10" dxfId="12" priority="6" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S31 H31:M31 A31:E31">
-    <cfRule type="top10" dxfId="11" priority="5" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S33 H33:M33 A33:E33">
-    <cfRule type="top10" dxfId="10" priority="4" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S32 H32:M32 A32:E32">
-    <cfRule type="top10" dxfId="9" priority="3" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O123:AB123">
-    <cfRule type="top10" dxfId="8" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O124:AB124">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>